<commit_message>
final commit with excel changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/swag_data.xlsx
+++ b/src/test/resources/testdata/swag_data.xlsx
@@ -4,32 +4,34 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15150" windowHeight="5520"/>
+    <workbookView windowWidth="14630" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="Swag_Labs_Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:C4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>FirstName</t>
   </si>
   <si>
+    <t>John</t>
+  </si>
+  <si>
     <t>LastName</t>
   </si>
   <si>
+    <t>Smith</t>
+  </si>
+  <si>
     <t>ZipCode</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Smith</t>
+    <t>77676</t>
   </si>
   <si>
     <t>Locked User Message</t>
@@ -38,13 +40,28 @@
     <t>Epic sadface: Sorry, this user has been locked out.</t>
   </si>
   <si>
+    <t>Payment Information</t>
+  </si>
+  <si>
     <t>SauceCard #31337</t>
   </si>
   <si>
+    <t>Shipping Information</t>
+  </si>
+  <si>
     <t>FREE PONY EXPRESS DELIVERY!</t>
   </si>
   <si>
+    <t>Success Message</t>
+  </si>
+  <si>
     <t>THANK YOU FOR YOUR ORDER</t>
+  </si>
+  <si>
+    <t>Dropdown Value</t>
+  </si>
+  <si>
+    <t>hilo</t>
   </si>
 </sst>
 </file>
@@ -53,9 +70,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -72,6 +89,12 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -81,9 +104,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF202124"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -93,21 +117,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -119,13 +128,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -147,14 +149,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -170,9 +164,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -186,11 +210,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -203,21 +227,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,37 +256,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,7 +388,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,61 +406,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,67 +436,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,30 +447,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -481,13 +474,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,26 +528,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,152 +552,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -690,10 +707,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1015,72 +1032,80 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="7" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="18.6363636363636" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>77676</v>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>